<commit_message>
change 1.xlsx in branch2
</commit_message>
<xml_diff>
--- a/1.xlsx
+++ b/1.xlsx
@@ -331,12 +331,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>45345345</v>
+      </c>
+      <c r="B1">
+        <v>56756756</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>